<commit_message>
I2C master/slave comm; library skeletons
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddharth\Sid\Projects\Smart Cart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddharth\Sid\Projects\Smart Cart\smart-cart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>12V SLA Battery</t>
   </si>
@@ -50,9 +50,6 @@
     <t>208 oz-in (rated); 19 RPM (rated); 3.8 A (stall)</t>
   </si>
   <si>
-    <t>12V Motor</t>
-  </si>
-  <si>
     <t>Unit Weight (lbs)</t>
   </si>
   <si>
@@ -117,6 +114,12 @@
   </si>
   <si>
     <t>200mm</t>
+  </si>
+  <si>
+    <t>6V Motor</t>
+  </si>
+  <si>
+    <t>Pololu</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +514,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>6</v>
@@ -523,16 +526,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -540,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3">
         <v>37</v>
@@ -560,11 +563,11 @@
       </c>
       <c r="J2" s="7">
         <f>SUM(C:C)</f>
-        <v>143.5</v>
+        <v>165.87</v>
       </c>
       <c r="K2">
         <f>SUM(G:G)</f>
-        <v>9.3955479999999998</v>
+        <v>8.072773999999999</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -572,7 +575,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3">
         <v>13</v>
@@ -593,16 +596,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3">
-        <v>17.63</v>
+        <v>40</v>
       </c>
       <c r="D4" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -612,15 +615,15 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>2.6455479999999998</v>
+        <v>1.3227739999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3">
         <v>4.99</v>
@@ -629,7 +632,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <f>0.78</f>
@@ -642,10 +645,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="C6" s="3">
         <v>9.2899999999999991</v>
@@ -663,10 +666,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
         <v>4.5199999999999996</v>
@@ -681,10 +684,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3">
         <v>7.06</v>
@@ -699,10 +702,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="C9" s="3">
         <v>9.68</v>
@@ -717,10 +720,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
         <v>7.4</v>
@@ -729,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -738,10 +741,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3">
         <v>13.55</v>
@@ -750,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -759,10 +762,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3">
         <v>19.38</v>
@@ -771,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -854,15 +857,15 @@
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7" location="57655k11/=1eeja5n"/>
-    <hyperlink ref="A9" r:id="rId8" location="57655k31/=1eejat2"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10" location="1265K31"/>
-    <hyperlink ref="A12" r:id="rId11" location="1265K31"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6" location="57655k11/=1eeja5n"/>
+    <hyperlink ref="A9" r:id="rId7" location="57655k31/=1eejat2"/>
+    <hyperlink ref="A10" r:id="rId8"/>
+    <hyperlink ref="A11" r:id="rId9" location="1265K31"/>
+    <hyperlink ref="A12" r:id="rId10" location="1265K31"/>
+    <hyperlink ref="A4" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>

</xml_diff>